<commit_message>
Forgot to save Excel Task Sheet before initial commit.
</commit_message>
<xml_diff>
--- a/FenrisManor.xlsx
+++ b/FenrisManor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projects\FenrisManor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1B55F8D-4AD0-4705-B216-97209C55B1C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADBD264-F1A8-4991-B4BB-9CFA8DB1E7F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{130E93C0-4585-4DCA-BB1F-FB445E51F350}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Tasks to Complete &amp; Schedule</t>
   </si>
@@ -75,9 +75,6 @@
     <t xml:space="preserve">      Fire Bomb</t>
   </si>
   <si>
-    <t xml:space="preserve">      Boomerang</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Power-Ups</t>
   </si>
   <si>
@@ -157,6 +154,12 @@
   </si>
   <si>
     <t xml:space="preserve">      Screen Wipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Axe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Stopwatch(?)</t>
   </si>
 </sst>
 </file>
@@ -383,30 +386,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -418,12 +397,6 @@
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -454,6 +427,36 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -771,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F16966D-9A22-4AD2-8431-8135EB455170}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,76 +793,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="7">
         <v>43470</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="7">
         <v>43478</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="19"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
@@ -868,7 +871,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -877,7 +880,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -886,7 +889,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
@@ -894,8 +897,8 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>26</v>
+      <c r="A11" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
@@ -903,8 +906,8 @@
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>27</v>
+      <c r="A12" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
@@ -912,8 +915,8 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
-        <v>28</v>
+      <c r="A13" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -921,8 +924,8 @@
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
-        <v>29</v>
+      <c r="A14" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
@@ -930,8 +933,8 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>30</v>
+      <c r="A15" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
@@ -939,8 +942,8 @@
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>31</v>
+      <c r="A16" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
@@ -948,8 +951,8 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
-        <v>32</v>
+      <c r="A17" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
@@ -958,7 +961,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
@@ -967,7 +970,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
@@ -976,7 +979,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
@@ -985,7 +988,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
@@ -994,7 +997,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
@@ -1003,7 +1006,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
@@ -1012,7 +1015,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
@@ -1021,7 +1024,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
@@ -1050,41 +1053,41 @@
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+        <v>42</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="4"/>
@@ -1093,7 +1096,7 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="4"/>
@@ -1101,8 +1104,8 @@
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
-        <v>18</v>
+      <c r="A34" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="4"/>
@@ -1110,8 +1113,8 @@
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21" t="s">
-        <v>40</v>
+      <c r="A35" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="4"/>
@@ -1119,8 +1122,8 @@
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="21" t="s">
-        <v>41</v>
+      <c r="A36" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="4"/>
@@ -1128,110 +1131,119 @@
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="28"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="H50" s="23"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E51" s="23"/>
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="H51" s="13"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E52" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Updated Task Sheet with completed projects
</commit_message>
<xml_diff>
--- a/FenrisManor.xlsx
+++ b/FenrisManor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projects\FenrisManor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADBD264-F1A8-4991-B4BB-9CFA8DB1E7F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C290419-D137-4D10-BD8E-3D33A402602E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{130E93C0-4585-4DCA-BB1F-FB445E51F350}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Tasks to Complete &amp; Schedule</t>
   </si>
@@ -372,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -458,6 +458,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -776,14 +782,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F16966D-9A22-4AD2-8431-8135EB455170}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
@@ -873,10 +880,16 @@
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="32">
+        <v>43482</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">

</xml_diff>